<commit_message>
route code generate by api
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
   <si>
     <t>*Note</t>
   </si>
@@ -20,7 +20,7 @@
     <t>api_name</t>
   </si>
   <si>
-    <t>Api</t>
+    <t>*Api</t>
   </si>
   <si>
     <t>query</t>
@@ -38,13 +38,19 @@
     <t>missing</t>
   </si>
   <si>
-    <t>Args</t>
+    <t>*Args</t>
   </si>
   <si>
     <t>ops_org_id</t>
   </si>
   <si>
     <t>page_no</t>
+  </si>
+  <si>
+    <t>query1</t>
+  </si>
+  <si>
+    <t>xxx</t>
   </si>
   <si>
     <t>Args:</t>
@@ -57,7 +63,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -74,12 +80,17 @@
       <name val="Helvetica"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="12"/>
       <color indexed="8"/>
-      <name val="Arial"/>
+      <name val="Verdana"/>
     </font>
     <font>
-      <sz val="13"/>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
     </font>
@@ -121,24 +132,21 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1409,9 +1417,9 @@
         <v>1</v>
       </c>
       <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" ht="16" customHeight="1">
       <c r="A2" t="s" s="2">
@@ -1421,9 +1429,9 @@
         <v>3</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
     </row>
     <row r="3" ht="16" customHeight="1">
       <c r="A3" t="s" s="2">
@@ -1441,7 +1449,7 @@
       <c r="E3" t="s" s="2">
         <v>7</v>
       </c>
-      <c r="F3" s="4"/>
+      <c r="F3" s="3"/>
     </row>
     <row r="4" ht="16" customHeight="1">
       <c r="A4" t="s" s="2">
@@ -1459,10 +1467,10 @@
       <c r="E4" s="2">
         <v>110000</v>
       </c>
-      <c r="F4" s="4"/>
+      <c r="F4" s="3"/>
     </row>
     <row r="5" ht="16" customHeight="1">
-      <c r="A5" s="4"/>
+      <c r="A5" s="3"/>
       <c r="B5" t="s" s="2">
         <v>10</v>
       </c>
@@ -1475,55 +1483,87 @@
       <c r="E5" s="2">
         <v>10</v>
       </c>
-      <c r="F5" s="4"/>
+      <c r="F5" s="3"/>
     </row>
     <row r="6" ht="15.65" customHeight="1">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+      <c r="A6" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
     </row>
     <row r="7" ht="15.65" customHeight="1">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
+      <c r="A7" t="s" s="2">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s" s="2">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s" s="2">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="F7" s="3"/>
     </row>
     <row r="8" ht="15.65" customHeight="1">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+      <c r="A8" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="F8" s="3"/>
     </row>
     <row r="9" ht="15.65" customHeight="1">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
+      <c r="A9" s="3"/>
+      <c r="B9" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>10</v>
+      </c>
+      <c r="F9" s="3"/>
     </row>
     <row r="10" ht="15.65" customHeight="1">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
     </row>
     <row r="11" ht="15.65" customHeight="1">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1543,85 +1583,85 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="12.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.75" style="5" customWidth="1"/>
-    <col min="2" max="2" width="8.75" style="5" customWidth="1"/>
-    <col min="3" max="3" width="8.75" style="5" customWidth="1"/>
-    <col min="4" max="4" width="8.75" style="5" customWidth="1"/>
-    <col min="5" max="5" width="8.75" style="5" customWidth="1"/>
-    <col min="6" max="256" width="6" style="5" customWidth="1"/>
+    <col min="1" max="1" width="8.75" style="4" customWidth="1"/>
+    <col min="2" max="2" width="8.75" style="4" customWidth="1"/>
+    <col min="3" max="3" width="8.75" style="4" customWidth="1"/>
+    <col min="4" max="4" width="8.75" style="4" customWidth="1"/>
+    <col min="5" max="5" width="8.75" style="4" customWidth="1"/>
+    <col min="6" max="256" width="6" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="16" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
+        <v>13</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" ht="15.65" customHeight="1">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" ht="15.65" customHeight="1">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" ht="15.65" customHeight="1">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
     </row>
     <row r="5" ht="15.65" customHeight="1">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" ht="15.65" customHeight="1">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" ht="15.65" customHeight="1">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" ht="15.65" customHeight="1">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" ht="15.65" customHeight="1">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" ht="15.65" customHeight="1">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>